<commit_message>
Update Naming Plots Regression
</commit_message>
<xml_diff>
--- a/regression/Plots_PC2_2022-06-10/Regression_parameters.xlsx
+++ b/regression/Plots_PC2_2022-06-10/Regression_parameters.xlsx
@@ -786,7 +786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BH23"/>
+  <dimension ref="A1:BH18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2447,61 +2447,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL10" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR10" t="n">
-        <v>8.022762500015318</v>
-      </c>
-      <c r="AS10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ10" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB10" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC10" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BF10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH10" t="n">
-        <v>0.001022439445943031</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2622,61 +2567,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL11" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR11" t="n">
-        <v>6.303833333344865</v>
-      </c>
-      <c r="AS11" t="n">
-        <v>0.01252407407192035</v>
-      </c>
-      <c r="AT11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ11" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB11" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC11" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH11" t="n">
-        <v>0.0004445193288406019</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -2797,61 +2687,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL12" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS12" t="n">
-        <v>9.761540210764803e-17</v>
-      </c>
-      <c r="AT12" t="n">
-        <v>0.9999999998941522</v>
-      </c>
-      <c r="AU12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY12" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ12" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB12" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC12" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE12" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BF12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH12" t="n">
-        <v>6.897278538017803e+91</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -2972,61 +2807,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL13" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR13" t="n">
-        <v>7.356957143920763</v>
-      </c>
-      <c r="AS13" t="n">
-        <v>0.5383107134257654</v>
-      </c>
-      <c r="AT13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ13" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB13" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC13" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BF13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH13" t="n">
-        <v>6.869687146128601e-08</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -3147,61 +2927,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL14" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR14" t="n">
-        <v>6.992215608701573</v>
-      </c>
-      <c r="AS14" t="n">
-        <v>0.002664469982012033</v>
-      </c>
-      <c r="AT14" t="n">
-        <v>0.8171007908548514</v>
-      </c>
-      <c r="AU14" t="n">
-        <v>-0.002032640831025812</v>
-      </c>
-      <c r="AV14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ14" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB14" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC14" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH14" t="n">
-        <v>1.528955752927596e-08</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -3322,61 +3047,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL15" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS15" t="n">
-        <v>-5.907394694351708e-18</v>
-      </c>
-      <c r="AT15" t="n">
-        <v>0.9999998590582626</v>
-      </c>
-      <c r="AU15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV15" t="n">
-        <v>5.281848917153139e-18</v>
-      </c>
-      <c r="AW15" t="n">
-        <v>1.00000011310739</v>
-      </c>
-      <c r="AX15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ15" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB15" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC15" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BF15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH15" t="n">
-        <v>1.556144389163582e+88</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -3497,61 +3167,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL16" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT16" t="n">
-        <v>-45.92519191736918</v>
-      </c>
-      <c r="AU16" t="n">
-        <v>0.3189249438706193</v>
-      </c>
-      <c r="AV16" t="n">
-        <v>-27.90906612213172</v>
-      </c>
-      <c r="AW16" t="n">
-        <v>1.200754950793703</v>
-      </c>
-      <c r="AX16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ16" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB16" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC16" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF16" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BH16" t="n">
-        <v>5.807891274991834e+152</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -3672,61 +3287,6 @@
           <t>Drammen_Clay_4_PC2</t>
         </is>
       </c>
-      <c r="AL17" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR17" t="n">
-        <v>8.022762500015318</v>
-      </c>
-      <c r="AS17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ17" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB17" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC17" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BF17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH17" t="n">
-        <v>0.001022439445943031</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -3846,346 +3406,6 @@
         <is>
           <t>Drammen_Clay_4_PC2</t>
         </is>
-      </c>
-      <c r="AL18" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR18" t="n">
-        <v>6.303833333344865</v>
-      </c>
-      <c r="AS18" t="n">
-        <v>0.01252407407192035</v>
-      </c>
-      <c r="AT18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ18" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB18" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC18" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE18" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF18" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH18" t="n">
-        <v>0.0004445193288406019</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="AL19" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS19" t="n">
-        <v>9.761540210764803e-17</v>
-      </c>
-      <c r="AT19" t="n">
-        <v>0.9999999998941522</v>
-      </c>
-      <c r="AU19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY19" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ19" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB19" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC19" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE19" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BF19" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BH19" t="n">
-        <v>6.897278538017803e+91</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="AL20" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR20" t="n">
-        <v>7.356957143920763</v>
-      </c>
-      <c r="AS20" t="n">
-        <v>0.5383107134257654</v>
-      </c>
-      <c r="AT20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY20" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ20" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB20" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC20" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE20" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BF20" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH20" t="n">
-        <v>6.869687146128601e-08</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="AL21" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR21" t="n">
-        <v>6.992215608701573</v>
-      </c>
-      <c r="AS21" t="n">
-        <v>0.002664469982012033</v>
-      </c>
-      <c r="AT21" t="n">
-        <v>0.8171007908548514</v>
-      </c>
-      <c r="AU21" t="n">
-        <v>-0.002032640831025812</v>
-      </c>
-      <c r="AV21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AW21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY21" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ21" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB21" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC21" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF21" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH21" t="n">
-        <v>1.528955752927596e-08</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="AL22" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS22" t="n">
-        <v>-5.907394694351708e-18</v>
-      </c>
-      <c r="AT22" t="n">
-        <v>0.9999998590582626</v>
-      </c>
-      <c r="AU22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV22" t="n">
-        <v>5.281848917153139e-18</v>
-      </c>
-      <c r="AW22" t="n">
-        <v>1.00000011310739</v>
-      </c>
-      <c r="AX22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY22" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ22" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB22" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC22" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE22" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BF22" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BH22" t="n">
-        <v>1.556144389163582e+88</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="AL23" t="inlineStr">
-        <is>
-          <t>Pu</t>
-        </is>
-      </c>
-      <c r="AR23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT23" t="n">
-        <v>-45.92519191736918</v>
-      </c>
-      <c r="AU23" t="n">
-        <v>0.3189249438706193</v>
-      </c>
-      <c r="AV23" t="n">
-        <v>-27.90906612213172</v>
-      </c>
-      <c r="AW23" t="n">
-        <v>1.200754950793703</v>
-      </c>
-      <c r="AX23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY23" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ23" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB23" t="inlineStr">
-        <is>
-          <t>Su</t>
-        </is>
-      </c>
-      <c r="BC23" t="inlineStr">
-        <is>
-          <t>z_D</t>
-        </is>
-      </c>
-      <c r="BE23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="BF23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BH23" t="n">
-        <v>5.807891274991834e+152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>